<commit_message>
make a report excel
implement the report excel part.
</commit_message>
<xml_diff>
--- a/src/main/resources/exel/Manage.xlsx
+++ b/src/main/resources/exel/Manage.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e013e576aa07c75d/Documents/employee-manage-system/src/main/resources/exel/"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="39">
   <si>
     <t>이름</t>
   </si>
@@ -104,12 +104,64 @@
   </si>
   <si>
     <t>kanata</t>
+  </si>
+  <si>
+    <t>Test01</t>
+  </si>
+  <si>
+    <t>2024-08-03</t>
+  </si>
+  <si>
+    <t>2024-08-22</t>
+  </si>
+  <si>
+    <t>Test02</t>
+  </si>
+  <si>
+    <t>2024-09-03</t>
+  </si>
+  <si>
+    <t>2024-09-04</t>
+  </si>
+  <si>
+    <t>Seoyoung</t>
+  </si>
+  <si>
+    <t>030416</t>
+  </si>
+  <si>
+    <t>010-5718-4778</t>
+  </si>
+  <si>
+    <t>seoyoung.you@gmail.com</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>이메일이 맞는 지 모르겠음</t>
+  </si>
+  <si>
+    <t>Ayoung</t>
+  </si>
+  <si>
+    <t>010-5719-4778</t>
+  </si>
+  <si>
+    <t>이메일 부재</t>
+  </si>
+  <si>
+    <t>첫 프로젝트</t>
+  </si>
+  <si>
+    <t>알바 충원</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,7 +561,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA95C06-7A65-4B9E-B40B-20DA95F0278D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G4" sqref="A2:G4"/>
@@ -517,13 +569,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="77.875" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.375"/>
+    <col min="2" max="2" customWidth="true" style="1" width="13.25"/>
+    <col min="3" max="3" customWidth="true" style="1" width="20.25"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.5"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.125"/>
+    <col min="6" max="6" customWidth="true" style="1" width="14.375"/>
+    <col min="7" max="7" customWidth="true" style="1" width="77.875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
@@ -549,27 +601,73 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s" s="1">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s" s="1">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s" s="1">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="1">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s" s="1">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s" s="1">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -587,9 +685,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="42.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="64" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="3"/>
+    <col min="1" max="1" customWidth="true" style="3" width="42.125"/>
+    <col min="2" max="2" customWidth="true" style="3" width="64.0"/>
+    <col min="3" max="16384" style="3" width="9.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -600,11 +698,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s" s="3">
         <v>21</v>
       </c>
     </row>
@@ -615,7 +713,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDAF18B-F349-43D4-978F-E1B991A6C84A}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
@@ -623,7 +721,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="17.875" style="3"/>
+    <col min="1" max="16384" style="3" width="17.875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
@@ -643,6 +741,49 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="3">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="3">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>